<commit_message>
Se agrega sesión 11. Pauta ejecución proyecto y beginShape, función para planimetría.
</commit_message>
<xml_diff>
--- a/sesion11/pautaPrototipo.xlsx
+++ b/sesion11/pautaPrototipo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hacking/Desktop/_P5.js-repositorio/sesion11/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hacking/Desktop/P5.js-repositorio/sesion11/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -401,7 +401,7 @@
   <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -503,6 +503,12 @@
       <c r="A11" t="s">
         <v>7</v>
       </c>
+      <c r="H11">
+        <v>20</v>
+      </c>
+      <c r="J11">
+        <v>5</v>
+      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
@@ -512,14 +518,6 @@
         <v>20</v>
       </c>
       <c r="J12">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="H13">
-        <v>20</v>
-      </c>
-      <c r="J13">
         <v>10</v>
       </c>
     </row>

</xml_diff>